<commit_message>
Story and TPS update
</commit_message>
<xml_diff>
--- a/docs/Stories.xlsx
+++ b/docs/Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koob8\Documents\ScreenManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonah/Documents/TouchscreenInterface/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28111236-0621-4B86-8AD9-14666887CDEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0426419-E01D-564A-992D-378617A8F8FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{23E1906B-1CE6-414F-8235-72A9FA54ED2A}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="12220" xr2:uid="{23E1906B-1CE6-414F-8235-72A9FA54ED2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Week 1 Stories Table</t>
   </si>
@@ -44,9 +39,6 @@
     <t>% Complete</t>
   </si>
   <si>
-    <t>The customer can use an internet browser in a limited capacity to increase security</t>
-  </si>
-  <si>
     <t>The customer can view the available products in the vending machine</t>
   </si>
   <si>
@@ -56,9 +48,6 @@
     <t>The customer can transfer electronic money via credit / debit card</t>
   </si>
   <si>
-    <t>Advertisers can publish ads that are displayed on the screen</t>
-  </si>
-  <si>
     <t>When no customer is using the machine, products automatically scroll to display</t>
   </si>
   <si>
@@ -75,6 +64,72 @@
   </si>
   <si>
     <t>Matt Peter, Michael Riess, Jonah Kubath</t>
+  </si>
+  <si>
+    <t>Work flow</t>
+  </si>
+  <si>
+    <t>Release 2-----------------------------------</t>
+  </si>
+  <si>
+    <t>Abstract - introduction</t>
+  </si>
+  <si>
+    <t>Large touchscreen broken into 3 sections and what the sections are used for</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>vending machine</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>modify the vending machine</t>
+  </si>
+  <si>
+    <t>Advertisers</t>
+  </si>
+  <si>
+    <t>IT?</t>
+  </si>
+  <si>
+    <t>Quantitiy falls below a cutoff - notify someone</t>
+  </si>
+  <si>
+    <t>The customer can use  internet browser, in a limited capacity to increase security</t>
+  </si>
+  <si>
+    <t>Add popup for purchase confirmation</t>
+  </si>
+  <si>
+    <t>Name for e-currency</t>
+  </si>
+  <si>
+    <t>Ads that are displayed on the screen on the Ad Window</t>
+  </si>
+  <si>
+    <t>Touchscreen Kiosk Interface</t>
+  </si>
+  <si>
+    <t>Security - interface works properly, someone hacks in, dispenses free items</t>
+  </si>
+  <si>
+    <t>Configure computer to only allow ssh</t>
+  </si>
+  <si>
+    <t>Let's encrypt to run</t>
+  </si>
+  <si>
+    <t>Ubuntu secure / disable services</t>
+  </si>
+  <si>
+    <t>Ansible to configure the computer</t>
   </si>
 </sst>
 </file>
@@ -427,125 +482,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18C7E13-27B9-4F26-BFB6-6B0C8DF0D2D8}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
       </c>
       <c r="E5" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -554,55 +597,163 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
         <v>15</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>20</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Install npm / nodejs
The working installation instructions are located in docs/Operating System/OS setup.txt
</commit_message>
<xml_diff>
--- a/docs/Stories.xlsx
+++ b/docs/Stories.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonah/Documents/TouchscreenInterface/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0426419-E01D-564A-992D-378617A8F8FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623551AC-13C4-4E42-B7A7-111D75973678}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="12220" xr2:uid="{23E1906B-1CE6-414F-8235-72A9FA54ED2A}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" xr2:uid="{23E1906B-1CE6-414F-8235-72A9FA54ED2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>Week 1 Stories Table</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Ansible to configure the computer</t>
+  </si>
+  <si>
+    <t>09/29/2018 Stories Table</t>
   </si>
 </sst>
 </file>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18C7E13-27B9-4F26-BFB6-6B0C8DF0D2D8}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,39 +499,39 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>15</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>40</v>
@@ -667,93 +667,93 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
         <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>